<commit_message>
fix admin dashboard, fix login alert, fix import file (final)
</commit_message>
<xml_diff>
--- a/data/datastud.xlsx
+++ b/data/datastud.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansori San\Downloads\Documents\Perkuliahan RPL\Semester 4\Web Programming\tubes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DED36C2-81C0-44D6-9727-FA306DE0296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E0C9B9E-06FD-443F-9755-857EF889D759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>Dada</t>
-  </si>
-  <si>
-    <t>Didi</t>
-  </si>
-  <si>
-    <t>Dede</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="58">
   <si>
     <t>P</t>
   </si>
@@ -51,10 +42,163 @@
     <t>12-F</t>
   </si>
   <si>
-    <t>2020 - 2021</t>
-  </si>
-  <si>
     <t>Belum Lunas</t>
+  </si>
+  <si>
+    <t>10-A</t>
+  </si>
+  <si>
+    <t>10-B</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>2020-2021</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>10-C</t>
+  </si>
+  <si>
+    <t>10-D</t>
+  </si>
+  <si>
+    <t>11-A</t>
+  </si>
+  <si>
+    <t>10-E</t>
+  </si>
+  <si>
+    <t>12-A</t>
+  </si>
+  <si>
+    <t>11-B</t>
+  </si>
+  <si>
+    <t>11-D</t>
+  </si>
+  <si>
+    <t>11-C</t>
+  </si>
+  <si>
+    <t>11-E</t>
+  </si>
+  <si>
+    <t>12-B</t>
+  </si>
+  <si>
+    <t>12-D</t>
+  </si>
+  <si>
+    <t>12-C</t>
+  </si>
+  <si>
+    <t>12-E</t>
+  </si>
+  <si>
+    <t>Mikazuki</t>
+  </si>
+  <si>
+    <t>Abe</t>
+  </si>
+  <si>
+    <t>Ogata</t>
+  </si>
+  <si>
+    <t>Chizuru</t>
+  </si>
+  <si>
+    <t>Anya</t>
+  </si>
+  <si>
+    <t>Yor</t>
+  </si>
+  <si>
+    <t>Loid</t>
+  </si>
+  <si>
+    <t>Kazuto</t>
+  </si>
+  <si>
+    <t>Tsukihime</t>
+  </si>
+  <si>
+    <t>Shin</t>
+  </si>
+  <si>
+    <t>Shiba</t>
+  </si>
+  <si>
+    <t>Mafu</t>
+  </si>
+  <si>
+    <t>Uzuru</t>
+  </si>
+  <si>
+    <t>Izann</t>
+  </si>
+  <si>
+    <t>Yuri</t>
+  </si>
+  <si>
+    <t>Rei</t>
+  </si>
+  <si>
+    <t>Kazuma</t>
+  </si>
+  <si>
+    <t>Megumin</t>
+  </si>
+  <si>
+    <t>Shintaro</t>
+  </si>
+  <si>
+    <t>Asuna</t>
+  </si>
+  <si>
+    <t>Yuuto</t>
+  </si>
+  <si>
+    <t>Oreki</t>
+  </si>
+  <si>
+    <t>Mayu</t>
+  </si>
+  <si>
+    <t>Kurumi</t>
+  </si>
+  <si>
+    <t>Saitama</t>
+  </si>
+  <si>
+    <t>Odama</t>
+  </si>
+  <si>
+    <t>Oguro</t>
+  </si>
+  <si>
+    <t>Lola</t>
+  </si>
+  <si>
+    <t>Bojji</t>
+  </si>
+  <si>
+    <t>Yukihime</t>
+  </si>
+  <si>
+    <t>Kurama</t>
+  </si>
+  <si>
+    <t>Asano</t>
+  </si>
+  <si>
+    <t>Ruri</t>
+  </si>
+  <si>
+    <t>Tohsaka</t>
   </si>
 </sst>
 </file>
@@ -62,7 +206,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -117,7 +261,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,19 +557,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>202020</v>
+        <v>200453</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1">
         <v>250000</v>
@@ -434,24 +578,24 @@
         <v>44727</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>212121</v>
+        <v>234545</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1">
         <v>250000</v>
@@ -460,24 +604,24 @@
         <v>44727</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>222222</v>
+        <v>232525</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
         <v>250000</v>
@@ -486,7 +630,813 @@
         <v>44727</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>224455</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>44728</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>225325</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G5" s="2">
+        <v>44729</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>221322</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G6" s="2">
+        <v>44730</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>241241</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G7" s="2">
+        <v>44731</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>222241</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G8" s="2">
+        <v>44732</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>231312</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G9" s="2">
+        <v>44733</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>234243</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>44734</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>214189</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>44735</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>224230</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G12" s="2">
+        <v>44736</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>244546</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G13" s="2">
+        <v>44737</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>233345</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G14" s="2">
+        <v>44738</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>222345</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G15" s="2">
+        <v>44739</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>289643</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G16" s="2">
+        <v>44740</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>234455</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G17" s="2">
+        <v>44741</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>233335</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G18" s="2">
+        <v>44742</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>234567</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G19" s="2">
+        <v>44713</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>234457</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G20" s="2">
+        <v>44714</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>223556</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G21" s="2">
+        <v>44715</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>298087</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G22" s="2">
+        <v>44716</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>276450</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G23" s="2">
+        <v>44717</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>267880</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G24" s="2">
+        <v>44718</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>276976</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G25" s="2">
+        <v>44719</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>287869</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G26" s="2">
+        <v>44720</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>287868</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G27" s="2">
+        <v>44721</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>286759</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G28" s="2">
+        <v>44722</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>278886</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G29" s="2">
+        <v>44723</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>234567</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G30" s="2">
+        <v>44724</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>265875</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G31" s="2">
+        <v>44725</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>255666</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G32" s="2">
+        <v>44726</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>243443</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G33" s="2">
+        <v>44727</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>223412</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="1">
+        <v>250000</v>
+      </c>
+      <c r="G34" s="2">
+        <v>44728</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>